<commit_message>
passed home page test methods
</commit_message>
<xml_diff>
--- a/src/main/java/com/automationpractice/qa/testdata/testdata.xlsx
+++ b/src/main/java/com/automationpractice/qa/testdata/testdata.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bec03fa0386512cb/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0290ACD0-D01B-4716-AECE-FA281001D17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{710AA077-4565-4831-B36E-A334A6289C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{BFDC4655-D4E8-4779-B86D-E2B1E87847E6}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23304" windowHeight="13224" xr2:uid="{BFDC4655-D4E8-4779-B86D-E2B1E87847E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>password</t>
   </si>
@@ -41,6 +37,9 @@
   </si>
   <si>
     <t>summer dress</t>
+  </si>
+  <si>
+    <t>search data</t>
   </si>
 </sst>
 </file>
@@ -64,12 +63,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,9 +90,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92E3C58-2995-4632-AB34-14EBF7F94087}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,12 +421,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>